<commit_message>
Interface and documentary changes.
git-svn-id: http://svnint.ou.nl:8080/svn/ADL/trunk@3138 80d59baa-9aef-c140-ba76-e18f3b6eea4d
</commit_message>
<xml_diff>
--- a/EURent/EURent-Demo.xlsx
+++ b/EURent/EURent-Demo.xlsx
@@ -336,11 +336,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -645,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,6 +1073,7 @@
       <c r="C35" t="s">
         <v>19</v>
       </c>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -1281,13 +1283,13 @@
       <c r="B49" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="3">
-        <f ca="1">TODAY() - 14</f>
-        <v>41786</v>
-      </c>
-      <c r="D49" s="3">
-        <f ca="1">TODAY()+3</f>
-        <v>41803</v>
+      <c r="C49" s="3" t="str">
+        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
+        <v>28-05-2014</v>
+      </c>
+      <c r="D49" s="3" t="str">
+        <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
+        <v>28-05-2014</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Interfaces voorzien van 'signaling' - mogelijkheid om 'todays date' op een vooraf ingestelde default waarde te zetten.
git-svn-id: http://svnint.ou.nl:8080/svn/ADL/trunk@3166 80d59baa-9aef-c140-ba76-e18f3b6eea4d
</commit_message>
<xml_diff>
--- a/EURent/EURent-Demo.xlsx
+++ b/EURent/EURent-Demo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>maxRentalDuration</t>
   </si>
@@ -207,9 +207,6 @@
     <t>contractedPickupBranch</t>
   </si>
   <si>
-    <t>contractedDropoffBranch</t>
-  </si>
-  <si>
     <t>rcAssignedCar</t>
   </si>
   <si>
@@ -264,7 +261,10 @@
     <t>RC_AMS_123</t>
   </si>
   <si>
-    <t>validDrivingLicense</t>
+    <t>contractedDropOffBranch</t>
+  </si>
+  <si>
+    <t>rcDrivingLicense</t>
   </si>
 </sst>
 </file>
@@ -644,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N49"/>
+  <dimension ref="A2:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:D48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,7 +798,8 @@
         <v>60</v>
       </c>
       <c r="E15">
-        <v>38</v>
+        <f>MAX(15,FLOOR($D15/2.1415,1))</f>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -815,7 +816,8 @@
         <v>25</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <f t="shared" ref="E16:E18" si="0">MAX(15,FLOOR($D16/2.1415,1))</f>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -832,7 +834,8 @@
         <v>34</v>
       </c>
       <c r="E17">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -846,10 +849,11 @@
         <v>35</v>
       </c>
       <c r="D18">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E18">
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -901,13 +905,13 @@
         <v>61</v>
       </c>
       <c r="E22">
-        <f>D22</f>
-        <v>61</v>
+        <f>MAX(33,FLOOR($D22*1.3,1))</f>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f t="shared" ref="A23:A27" si="0">CONCATENATE($B23,"-",$C23)</f>
+        <f t="shared" ref="A23:A27" si="1">CONCATENATE($B23,"-",$C23)</f>
         <v>AMS-RTD</v>
       </c>
       <c r="B23" t="s">
@@ -920,13 +924,13 @@
         <v>67</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:E27" si="1">D23</f>
-        <v>67</v>
+        <f t="shared" ref="E23:E27" si="2">MAX(33,FLOOR($D23*1.3,1))</f>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>AMS-UTR</v>
       </c>
       <c r="B24" t="s">
@@ -939,13 +943,13 @@
         <v>38</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
-        <v>38</v>
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DHG-RTD</v>
       </c>
       <c r="B25" t="s">
@@ -958,13 +962,13 @@
         <v>23</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DHG-UTR</v>
       </c>
       <c r="B26" t="s">
@@ -977,13 +981,13 @@
         <v>63</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
-        <v>63</v>
+        <f t="shared" si="2"/>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>RTD-UTR</v>
       </c>
       <c r="B27" t="s">
@@ -996,8 +1000,8 @@
         <v>56</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
-        <v>56</v>
+        <f t="shared" si="2"/>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1041,7 +1045,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1063,7 +1067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1075,7 +1079,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1097,7 +1101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -1119,31 +1123,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
@@ -1160,34 +1155,37 @@
         <v>62</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M46" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
@@ -1195,10 +1193,10 @@
         <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>7</v>
@@ -1210,28 +1208,31 @@
         <v>44</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M47" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="N47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O47" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -1254,42 +1255,45 @@
         <v>53</v>
       </c>
       <c r="H48" t="s">
+        <v>78</v>
+      </c>
+      <c r="I48" t="s">
+        <v>77</v>
+      </c>
+      <c r="J48" t="s">
+        <v>76</v>
+      </c>
+      <c r="K48" t="s">
         <v>79</v>
       </c>
-      <c r="I48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J48" t="s">
-        <v>80</v>
-      </c>
-      <c r="K48" t="s">
-        <v>80</v>
-      </c>
-      <c r="L48" t="str">
+      <c r="L48" t="s">
+        <v>79</v>
+      </c>
+      <c r="M48" t="str">
         <f>$G48</f>
         <v>3-RTD-18</v>
       </c>
-      <c r="M48" s="3">
+      <c r="N48" s="3">
         <v>41769</v>
       </c>
-      <c r="N48" t="s">
+      <c r="O48" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="3" t="str">
         <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
-        <v>28-05-2014</v>
+        <v>05-06-2014</v>
       </c>
       <c r="D49" s="3" t="str">
         <f ca="1">TEXT((TODAY()-14),"DD-MM-JJJJ")</f>
-        <v>28-05-2014</v>
+        <v>05-06-2014</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
@@ -1301,18 +1305,21 @@
         <v>47</v>
       </c>
       <c r="H49" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" t="s">
+        <v>77</v>
+      </c>
+      <c r="J49" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" t="s">
         <v>79</v>
       </c>
-      <c r="I49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J49" t="s">
-        <v>80</v>
-      </c>
-      <c r="K49" t="s">
-        <v>80</v>
-      </c>
-      <c r="M49" s="3"/>
+      <c r="L49" t="s">
+        <v>79</v>
+      </c>
+      <c r="N49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>